<commit_message>
minor changes in spanish templates
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/spanisch.xlsx
+++ b/src/spz/templates/export/spanisch.xlsx
@@ -21,9 +21,6 @@
     <sheet name="Teilnehmer" sheetId="13" r:id="rId7"/>
     <sheet name="Einstellungen" sheetId="14" r:id="rId8"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <definedNames>
     <definedName name="DOZENT">OFFSET(Einstellungen!$F$2,,,COUNTIF(Einstellungen!$F$2:$F$18,"&gt;"""),)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Extrapunkte!$A$1:$K$30</definedName>
@@ -1035,63 +1032,63 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1424,39 +1421,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="RAWDATA"/>
-      <sheetName val="Notenliste"/>
-      <sheetName val="Extrapunkte"/>
-      <sheetName val="Notenverteilung"/>
-      <sheetName val="Printlist"/>
-      <sheetName val="Paricipantlist"/>
-      <sheetName val="Teilnehmer"/>
-      <sheetName val="Einstellungen"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>course.name</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3993,12 +3957,12 @@
         <v>63</v>
       </c>
       <c r="C31" s="23"/>
-      <c r="D31" s="93" t="s">
+      <c r="D31" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
+      <c r="E31" s="95"/>
+      <c r="F31" s="95"/>
+      <c r="G31" s="95"/>
       <c r="H31" s="31"/>
       <c r="I31" s="25"/>
       <c r="J31" s="31"/>
@@ -4013,10 +3977,10 @@
         <v>106</v>
       </c>
       <c r="C32" s="23"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="93"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="95"/>
+      <c r="G32" s="95"/>
       <c r="H32" s="31"/>
       <c r="I32" s="25"/>
       <c r="J32" s="31"/>
@@ -4031,10 +3995,10 @@
         <v>107</v>
       </c>
       <c r="C33" s="23"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="95"/>
+      <c r="G33" s="95"/>
       <c r="H33" s="31"/>
       <c r="I33" s="25"/>
       <c r="J33" s="31"/>
@@ -4049,10 +4013,10 @@
         <v>110</v>
       </c>
       <c r="C34" s="23"/>
-      <c r="D34" s="93"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="93"/>
+      <c r="D34" s="95"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="95"/>
       <c r="H34" s="31"/>
       <c r="I34" s="25"/>
       <c r="J34" s="31"/>
@@ -4067,10 +4031,10 @@
         <v>111</v>
       </c>
       <c r="C35" s="23"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="95"/>
       <c r="H35" s="31"/>
       <c r="I35" s="25"/>
       <c r="J35" s="31"/>
@@ -4085,10 +4049,10 @@
         <v>108</v>
       </c>
       <c r="C36" s="23"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="93"/>
-      <c r="G36" s="93"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="95"/>
       <c r="H36" s="31"/>
       <c r="I36" s="25"/>
       <c r="J36" s="31"/>
@@ -4103,10 +4067,10 @@
         <v>109</v>
       </c>
       <c r="C37" s="23"/>
-      <c r="D37" s="93"/>
-      <c r="E37" s="93"/>
-      <c r="F37" s="93"/>
-      <c r="G37" s="93"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="95"/>
+      <c r="G37" s="95"/>
       <c r="H37" s="22"/>
       <c r="I37" s="25"/>
       <c r="J37" s="22"/>
@@ -4193,7 +4157,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4210,16 +4174,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="str">
-        <f>[1]Notenliste!B34</f>
+      <c r="A1" s="93" t="str">
+        <f>Notenliste!B34</f>
         <v>course.name</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
       <c r="I1" s="82"/>
       <c r="J1" s="92" t="s">
         <v>120</v>
@@ -4283,7 +4247,7 @@
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
-      <c r="I3" s="112">
+      <c r="I3" s="94">
         <f>SUM(E3:H3)</f>
         <v>0</v>
       </c>
@@ -4315,7 +4279,7 @@
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
-      <c r="I4" s="112">
+      <c r="I4" s="94">
         <f t="shared" ref="I4:I27" si="0">SUM(E4:H4)</f>
         <v>0</v>
       </c>
@@ -4347,7 +4311,7 @@
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
-      <c r="I5" s="112">
+      <c r="I5" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4379,7 +4343,7 @@
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
-      <c r="I6" s="112">
+      <c r="I6" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4411,7 +4375,7 @@
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
-      <c r="I7" s="112">
+      <c r="I7" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4443,7 +4407,7 @@
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
-      <c r="I8" s="112">
+      <c r="I8" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4475,7 +4439,7 @@
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
-      <c r="I9" s="112">
+      <c r="I9" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4507,7 +4471,7 @@
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="112">
+      <c r="I10" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4539,7 +4503,7 @@
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
-      <c r="I11" s="112">
+      <c r="I11" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4571,7 +4535,7 @@
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
-      <c r="I12" s="112">
+      <c r="I12" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4603,7 +4567,7 @@
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
-      <c r="I13" s="112">
+      <c r="I13" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4635,7 +4599,7 @@
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
-      <c r="I14" s="112">
+      <c r="I14" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4667,7 +4631,7 @@
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
-      <c r="I15" s="112">
+      <c r="I15" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4699,7 +4663,7 @@
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
       <c r="H16" s="34"/>
-      <c r="I16" s="112">
+      <c r="I16" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4731,7 +4695,7 @@
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
-      <c r="I17" s="112">
+      <c r="I17" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4763,7 +4727,7 @@
       <c r="F18" s="34"/>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
-      <c r="I18" s="112">
+      <c r="I18" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4795,7 +4759,7 @@
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
-      <c r="I19" s="112">
+      <c r="I19" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4827,7 +4791,7 @@
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
-      <c r="I20" s="112">
+      <c r="I20" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4859,7 +4823,7 @@
       <c r="F21" s="34"/>
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
-      <c r="I21" s="112">
+      <c r="I21" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4891,7 +4855,7 @@
       <c r="F22" s="34"/>
       <c r="G22" s="34"/>
       <c r="H22" s="34"/>
-      <c r="I22" s="112">
+      <c r="I22" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4923,7 +4887,7 @@
       <c r="F23" s="34"/>
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
-      <c r="I23" s="112">
+      <c r="I23" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4955,7 +4919,7 @@
       <c r="F24" s="34"/>
       <c r="G24" s="34"/>
       <c r="H24" s="34"/>
-      <c r="I24" s="112">
+      <c r="I24" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4987,7 +4951,7 @@
       <c r="F25" s="34"/>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
-      <c r="I25" s="112">
+      <c r="I25" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5019,7 +4983,7 @@
       <c r="F26" s="34"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
-      <c r="I26" s="112">
+      <c r="I26" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5051,7 +5015,7 @@
       <c r="F27" s="34"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="112">
+      <c r="I27" s="94">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5164,11 +5128,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="str">
+      <c r="A1" s="97" t="str">
         <f>Notenliste!B34</f>
         <v>course.name</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="97"/>
       <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
@@ -5325,45 +5289,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="61" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="str">
+      <c r="A1" s="98" t="str">
         <f>Notenliste!B34&amp;" / "&amp;Notenliste!B35</f>
         <v>course.name / course.name_english</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
     </row>
     <row r="2" spans="1:14" s="61" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="str">
+      <c r="A2" s="99" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B31</f>
         <v>Dozent/in: Elena Moya Royo</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="98" t="str">
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="100" t="str">
         <f>"Semster: "&amp;Notenliste!B36</f>
         <v>Semster: semester</v>
       </c>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
     </row>
     <row r="3" spans="1:14" s="62" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -6857,86 +6821,86 @@
       <c r="N29" s="60"/>
     </row>
     <row r="30" spans="1:14" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="99" t="s">
+      <c r="A30" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="99"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="99"/>
-      <c r="G30" s="99"/>
-      <c r="H30" s="99"/>
-      <c r="I30" s="99"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="99"/>
-      <c r="M30" s="99"/>
-      <c r="N30" s="99"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="101"/>
+      <c r="H30" s="101"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="101"/>
+      <c r="K30" s="101"/>
+      <c r="L30" s="101"/>
+      <c r="M30" s="101"/>
+      <c r="N30" s="101"/>
     </row>
     <row r="31" spans="1:14" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="99"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="99"/>
-      <c r="L31" s="99"/>
-      <c r="M31" s="99"/>
-      <c r="N31" s="99"/>
+      <c r="A31" s="101"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="101"/>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
+      <c r="K31" s="101"/>
+      <c r="L31" s="101"/>
+      <c r="M31" s="101"/>
+      <c r="N31" s="101"/>
     </row>
     <row r="32" spans="1:14" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="99"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="99"/>
-      <c r="D32" s="99"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="99"/>
-      <c r="G32" s="99"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="99"/>
-      <c r="K32" s="99"/>
-      <c r="L32" s="99"/>
-      <c r="M32" s="99"/>
-      <c r="N32" s="99"/>
+      <c r="A32" s="101"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="101"/>
+      <c r="I32" s="101"/>
+      <c r="J32" s="101"/>
+      <c r="K32" s="101"/>
+      <c r="L32" s="101"/>
+      <c r="M32" s="101"/>
+      <c r="N32" s="101"/>
     </row>
     <row r="33" spans="1:15" s="61" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="99"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="99"/>
-      <c r="M33" s="99"/>
-      <c r="N33" s="99"/>
+      <c r="A33" s="101"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="101"/>
+      <c r="H33" s="101"/>
+      <c r="I33" s="101"/>
+      <c r="J33" s="101"/>
+      <c r="K33" s="101"/>
+      <c r="L33" s="101"/>
+      <c r="M33" s="101"/>
+      <c r="N33" s="101"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="99"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="99"/>
-      <c r="J34" s="99"/>
-      <c r="K34" s="99"/>
-      <c r="L34" s="99"/>
-      <c r="M34" s="99"/>
-      <c r="N34" s="99"/>
+      <c r="A34" s="101"/>
+      <c r="B34" s="101"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="101"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="101"/>
+      <c r="J34" s="101"/>
+      <c r="K34" s="101"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="101"/>
+      <c r="N34" s="101"/>
       <c r="O34" s="61"/>
     </row>
   </sheetData>
@@ -6991,105 +6955,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="str">
+      <c r="A1" s="104" t="str">
         <f>Notenliste!B34&amp;" / "&amp;Notenliste!B35</f>
         <v>course.name / course.name_english</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="104"/>
+      <c r="Q1" s="104"/>
+      <c r="R1" s="104"/>
+      <c r="S1" s="104"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="104"/>
+      <c r="V1" s="104"/>
+      <c r="W1" s="104"/>
+      <c r="X1" s="104"/>
     </row>
     <row r="2" spans="1:24" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="102"/>
-      <c r="T2" s="102"/>
-      <c r="U2" s="102"/>
-      <c r="V2" s="102"/>
-      <c r="W2" s="102"/>
-      <c r="X2" s="102"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="103" t="str">
+      <c r="A3" s="105" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B31</f>
         <v>Dozent/in: Elena Moya Royo</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
       <c r="F3" s="43"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
-      <c r="P3" s="104"/>
-      <c r="Q3" s="104"/>
-      <c r="R3" s="104"/>
-      <c r="S3" s="104"/>
-      <c r="T3" s="104"/>
-      <c r="U3" s="104"/>
-      <c r="V3" s="104"/>
-      <c r="W3" s="104"/>
-      <c r="X3" s="104"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="106"/>
+      <c r="O3" s="106"/>
+      <c r="P3" s="106"/>
+      <c r="Q3" s="106"/>
+      <c r="R3" s="106"/>
+      <c r="S3" s="106"/>
+      <c r="T3" s="106"/>
+      <c r="U3" s="106"/>
+      <c r="V3" s="106"/>
+      <c r="W3" s="106"/>
+      <c r="X3" s="106"/>
     </row>
     <row r="4" spans="1:24" s="16" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="107" t="s">
+      <c r="E4" s="109" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="44"/>
@@ -7108,22 +7072,22 @@
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
       <c r="U4" s="46"/>
-      <c r="V4" s="109" t="s">
+      <c r="V4" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="W4" s="100" t="s">
+      <c r="W4" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="X4" s="100" t="s">
+      <c r="X4" s="102" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="106"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="108"/>
+      <c r="A5" s="108"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="110"/>
       <c r="F5" s="47"/>
       <c r="G5" s="45">
         <v>1</v>
@@ -7168,9 +7132,9 @@
         <v>14</v>
       </c>
       <c r="U5" s="48"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="101"/>
-      <c r="X5" s="101"/>
+      <c r="V5" s="112"/>
+      <c r="W5" s="103"/>
+      <c r="X5" s="103"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="17">

</xml_diff>

<commit_message>
update spanish export templates for SS24
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/spanisch.xlsx
+++ b/src/spz/templates/export/spanisch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="11" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>mündliche Beteiligung</t>
+  </si>
+  <si>
+    <t>Gabriela Fahra</t>
+  </si>
+  <si>
+    <t>Lucía Serres</t>
   </si>
 </sst>
 </file>
@@ -775,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1090,6 +1096,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1996,8 +2004,8 @@
   </sheetPr>
   <dimension ref="A1:WVW59"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4156,7 +4164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -8697,10 +8705,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8742,7 +8750,7 @@
       <c r="D2" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="80" t="s">
         <v>63</v>
       </c>
       <c r="H2" s="72" t="s">
@@ -8806,8 +8814,8 @@
       <c r="D6" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="71" t="s">
-        <v>82</v>
+      <c r="F6" s="113" t="s">
+        <v>123</v>
       </c>
       <c r="H6" s="73"/>
     </row>
@@ -8822,7 +8830,7 @@
         <v>74</v>
       </c>
       <c r="F7" s="71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H7" s="73"/>
     </row>
@@ -8837,7 +8845,7 @@
         <v>95</v>
       </c>
       <c r="F8" s="71" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="H8" s="73"/>
     </row>
@@ -8852,7 +8860,7 @@
         <v>96</v>
       </c>
       <c r="F9" s="71" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="H9" s="73"/>
     </row>
@@ -8863,7 +8871,7 @@
         <v>75</v>
       </c>
       <c r="F10" s="71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H10" s="73"/>
     </row>
@@ -8874,7 +8882,7 @@
         <v>76</v>
       </c>
       <c r="F11" s="71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H11" s="73"/>
     </row>
@@ -8885,7 +8893,7 @@
         <v>90</v>
       </c>
       <c r="F12" s="71" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" s="73"/>
     </row>
@@ -8896,7 +8904,7 @@
         <v>91</v>
       </c>
       <c r="F13" s="71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H13" s="73"/>
     </row>
@@ -8907,7 +8915,7 @@
         <v>92</v>
       </c>
       <c r="F14" s="71" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="H14" s="73"/>
     </row>
@@ -8918,7 +8926,7 @@
         <v>62</v>
       </c>
       <c r="F15" s="71" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="H15" s="73"/>
     </row>
@@ -8929,7 +8937,7 @@
         <v>93</v>
       </c>
       <c r="F16" s="71" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="H16" s="73"/>
     </row>
@@ -8937,15 +8945,25 @@
       <c r="A17" s="71"/>
       <c r="B17" s="71"/>
       <c r="D17" s="71"/>
-      <c r="F17" s="71"/>
+      <c r="F17" s="71" t="s">
+        <v>112</v>
+      </c>
       <c r="H17" s="73"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="74"/>
       <c r="B18" s="74"/>
       <c r="D18" s="74"/>
-      <c r="F18" s="74"/>
+      <c r="F18" s="74" t="s">
+        <v>124</v>
+      </c>
       <c r="H18" s="75"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="114"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="114"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>